<commit_message>
Count Even and Odd
</commit_message>
<xml_diff>
--- a/Problem.xlsx
+++ b/Problem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\Amcat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A10410-C5DC-4069-9D4A-C9F48CE49097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB36DCA-EE7F-4D71-8D17-524445D1101E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -488,7 +488,7 @@
   <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -559,12 +559,12 @@
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rotate array by k left
</commit_message>
<xml_diff>
--- a/Problem.xlsx
+++ b/Problem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\Amcat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB36DCA-EE7F-4D71-8D17-524445D1101E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831C3D0E-B04A-4E93-B6C9-9D68248904F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,12 +569,12 @@
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Best time to buy and sell stock
</commit_message>
<xml_diff>
--- a/Problem.xlsx
+++ b/Problem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\Amcat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD39CFAB-DE0E-445C-9647-0B8D24F836B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A671CDD-7BEF-4A99-9D48-FD3C82B67C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -614,12 +614,12 @@
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solved some more problems
</commit_message>
<xml_diff>
--- a/Problem.xlsx
+++ b/Problem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\Amcat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B8C341-5FAD-46B7-8BB1-4EA085822319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31975566-A877-44BE-83E7-1A8CB041C481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,12 +179,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,10 +195,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,12 +542,12 @@
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>